<commit_message>
1214-add bigdata study path file
</commit_message>
<xml_diff>
--- a/极客时间-智能采集-基础信息.xlsx
+++ b/极客时间-智能采集-基础信息.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A243D30-1AFA-8248-A336-92A8DA30935F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31080" yWindow="2160" windowWidth="27800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31080" yWindow="2160" windowWidth="27804" windowHeight="17544"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -1361,10 +1360,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+    <numFmt numFmtId="176" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1425,8 +1424,8 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1767,31 +1766,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
     <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="7.5" style="1" customWidth="1"/>
+    <col min="3" max="4" width="7.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="39.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="39.44140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="1"/>
+    <col min="10" max="10" width="9.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2175,7 +2173,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1">
+    <row r="16" spans="1:12">
       <c r="B16" s="1" t="s">
         <v>416</v>
       </c>
@@ -3129,7 +3127,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="2:12" hidden="1">
+    <row r="55" spans="2:12">
       <c r="B55" s="1" t="s">
         <v>416</v>
       </c>
@@ -3227,7 +3225,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="2:12" hidden="1">
+    <row r="59" spans="2:12">
       <c r="B59" s="1" t="s">
         <v>416</v>
       </c>
@@ -3276,7 +3274,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="2:12" hidden="1">
+    <row r="61" spans="2:12">
       <c r="B61" s="1" t="s">
         <v>395</v>
       </c>
@@ -3351,7 +3349,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="2:12" hidden="1">
+    <row r="64" spans="2:12">
       <c r="B64" s="1" t="s">
         <v>395</v>
       </c>
@@ -3383,7 +3381,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="2:12" hidden="1">
+    <row r="65" spans="2:12">
       <c r="B65" s="1" t="s">
         <v>416</v>
       </c>
@@ -3409,7 +3407,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="2:12" hidden="1">
+    <row r="66" spans="2:12">
       <c r="B66" s="1" t="s">
         <v>395</v>
       </c>
@@ -3464,7 +3462,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="2:12" hidden="1">
+    <row r="68" spans="2:12">
       <c r="B68" s="1" t="s">
         <v>393</v>
       </c>
@@ -3493,7 +3491,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="2:12" hidden="1">
+    <row r="69" spans="2:12">
       <c r="B69" s="1" t="s">
         <v>416</v>
       </c>
@@ -3525,7 +3523,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="2:12" hidden="1">
+    <row r="70" spans="2:12">
       <c r="B70" s="1" t="s">
         <v>416</v>
       </c>
@@ -3551,7 +3549,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="2:12" hidden="1">
+    <row r="71" spans="2:12">
       <c r="B71" s="1" t="s">
         <v>395</v>
       </c>
@@ -3580,7 +3578,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="2:12" hidden="1">
+    <row r="72" spans="2:12">
       <c r="B72" s="1" t="s">
         <v>418</v>
       </c>
@@ -3681,7 +3679,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="2:12" hidden="1">
+    <row r="76" spans="2:12">
       <c r="B76" s="1" t="s">
         <v>393</v>
       </c>
@@ -3736,7 +3734,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="2:12" hidden="1">
+    <row r="78" spans="2:12">
       <c r="B78" s="1" t="s">
         <v>418</v>
       </c>
@@ -3762,7 +3760,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="79" spans="2:12" hidden="1">
+    <row r="79" spans="2:12">
       <c r="B79" s="1" t="s">
         <v>416</v>
       </c>
@@ -3791,7 +3789,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="2:12" hidden="1">
+    <row r="80" spans="2:12">
       <c r="B80" s="1" t="s">
         <v>418</v>
       </c>
@@ -3817,7 +3815,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="81" spans="2:12" hidden="1">
+    <row r="81" spans="2:12">
       <c r="B81" s="1" t="s">
         <v>394</v>
       </c>
@@ -3892,7 +3890,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="2:12" hidden="1">
+    <row r="84" spans="2:12">
       <c r="B84" s="1" t="s">
         <v>393</v>
       </c>
@@ -3973,7 +3971,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="2:12" hidden="1">
+    <row r="87" spans="2:12">
       <c r="B87" s="1" t="s">
         <v>416</v>
       </c>
@@ -4005,7 +4003,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="2:12" hidden="1">
+    <row r="88" spans="2:12">
       <c r="B88" s="1" t="s">
         <v>395</v>
       </c>
@@ -4037,7 +4035,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="2:12" hidden="1">
+    <row r="89" spans="2:12">
       <c r="B89" s="1" t="s">
         <v>416</v>
       </c>
@@ -4063,7 +4061,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="90" spans="2:12" hidden="1">
+    <row r="90" spans="2:12">
       <c r="B90" s="1" t="s">
         <v>416</v>
       </c>
@@ -4089,7 +4087,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="2:12" hidden="1">
+    <row r="91" spans="2:12">
       <c r="B91" s="1" t="s">
         <v>416</v>
       </c>
@@ -4118,7 +4116,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="2:12" hidden="1">
+    <row r="92" spans="2:12">
       <c r="B92" s="1" t="s">
         <v>416</v>
       </c>
@@ -4144,7 +4142,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="93" spans="2:12" hidden="1">
+    <row r="93" spans="2:12">
       <c r="B93" s="1" t="s">
         <v>416</v>
       </c>
@@ -4173,7 +4171,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="94" spans="2:12" hidden="1">
+    <row r="94" spans="2:12">
       <c r="B94" s="1" t="s">
         <v>394</v>
       </c>
@@ -4248,7 +4246,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="2:12" hidden="1">
+    <row r="97" spans="2:12">
       <c r="B97" s="1" t="s">
         <v>416</v>
       </c>
@@ -4274,7 +4272,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="98" spans="2:12" hidden="1">
+    <row r="98" spans="2:12">
       <c r="B98" s="1" t="s">
         <v>416</v>
       </c>
@@ -4300,7 +4298,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="99" spans="2:12" hidden="1">
+    <row r="99" spans="2:12">
       <c r="B99" s="1" t="s">
         <v>395</v>
       </c>
@@ -4355,7 +4353,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="101" spans="2:12" hidden="1">
+    <row r="101" spans="2:12">
       <c r="B101" s="1" t="s">
         <v>416</v>
       </c>
@@ -4384,7 +4382,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="102" spans="2:12" hidden="1">
+    <row r="102" spans="2:12">
       <c r="B102" s="1" t="s">
         <v>393</v>
       </c>
@@ -4413,7 +4411,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="103" spans="2:12" hidden="1">
+    <row r="103" spans="2:12">
       <c r="B103" s="1" t="s">
         <v>395</v>
       </c>
@@ -4468,7 +4466,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="105" spans="2:12" hidden="1">
+    <row r="105" spans="2:12">
       <c r="B105" s="1" t="s">
         <v>394</v>
       </c>
@@ -4497,7 +4495,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="106" spans="2:12" hidden="1">
+    <row r="106" spans="2:12">
       <c r="B106" s="1" t="s">
         <v>418</v>
       </c>
@@ -4523,7 +4521,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="107" spans="2:12" hidden="1">
+    <row r="107" spans="2:12">
       <c r="B107" s="1" t="s">
         <v>416</v>
       </c>
@@ -4555,7 +4553,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="108" spans="2:12" hidden="1">
+    <row r="108" spans="2:12">
       <c r="B108" s="1" t="s">
         <v>395</v>
       </c>
@@ -4584,7 +4582,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="109" spans="2:12" hidden="1">
+    <row r="109" spans="2:12">
       <c r="B109" s="1" t="s">
         <v>418</v>
       </c>
@@ -4611,18 +4609,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:D109" xr:uid="{A85DAECB-B4B4-E847-92EC-C78FB355D5AF}">
-    <filterColumn colId="2">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:D109"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{0A0661DC-A8C9-2149-9C21-E45FAB300260}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
       <formula1>"后端 &amp; 架构,前端 &amp; 移动,CS专业课,AI &amp; 大数据,产品 &amp; 运营,运维 &amp; 测试,管理 &amp; 效率"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>